<commit_message>
payment + send invoice
</commit_message>
<xml_diff>
--- a/Appointment_List.xlsx
+++ b/Appointment_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaibi\eclipse-workspace\SC2002\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D765C7-1438-40C8-8F7C-DEAD7143DEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1106A947-39B5-418E-9B79-C5570C0E26C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{877EF473-33D4-4818-B04B-2D2C314AF0C4}"/>
+    <workbookView xWindow="5985" yWindow="810" windowWidth="21600" windowHeight="11295" xr2:uid="{877EF473-33D4-4818-B04B-2D2C314AF0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>APT ID</t>
   </si>
@@ -86,79 +86,46 @@
     <t>Alice Brown</t>
   </si>
   <si>
-    <t>2026-02-02 02:02</t>
+    <t>2027-03-05 10:00</t>
   </si>
   <si>
     <t>pending</t>
   </si>
   <si>
-    <t>cancelled</t>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>paid</t>
   </si>
   <si>
     <t>APT2</t>
   </si>
   <si>
-    <t>2025-03-03 10:30</t>
+    <t>2026-03-06 03:03</t>
+  </si>
+  <si>
+    <t>Price ($)</t>
+  </si>
+  <si>
+    <t>APT3</t>
+  </si>
+  <si>
+    <t>2028-03-03 10:00</t>
   </si>
   <si>
     <t>confirmed</t>
   </si>
   <si>
-    <t>APT3</t>
-  </si>
-  <si>
-    <t>2026-03-10 10:10</t>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>unpaid</t>
   </si>
   <si>
     <t>APT4</t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t>paid</t>
-  </si>
-  <si>
-    <t>APT5</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>APT6</t>
-  </si>
-  <si>
-    <t>2025-03-01 20:20</t>
-  </si>
-  <si>
-    <t>APT7</t>
-  </si>
-  <si>
-    <t>2025-06-07 03:03</t>
-  </si>
-  <si>
-    <t>APT8</t>
-  </si>
-  <si>
-    <t>2025-06-07 10:30</t>
-  </si>
-  <si>
-    <t>APT9</t>
-  </si>
-  <si>
-    <t>2027-06-03 10:30</t>
-  </si>
-  <si>
-    <t>APT10</t>
-  </si>
-  <si>
-    <t>2025-03-02 10:30</t>
-  </si>
-  <si>
-    <t>APT11</t>
-  </si>
-  <si>
-    <t>2026-03-10 10:30</t>
+    <t>2029-03-06 04:30</t>
   </si>
 </sst>
 </file>
@@ -531,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A6F2D2-9B8A-4EAD-AB99-BF9B532826C4}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +510,7 @@
     <col min="6" max="6" customWidth="true" width="24.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
@@ -577,8 +544,11 @@
       <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="0">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="0">
         <v>11</v>
       </c>
@@ -598,10 +568,22 @@
         <v>16</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
         <v>11</v>
       </c>
@@ -609,7 +591,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>14</v>
@@ -618,10 +600,22 @@
         <v>15</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -632,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>14</v>
@@ -641,22 +635,25 @@
         <v>15</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s" s="0">
         <v>17</v>
+      </c>
+      <c r="L4" t="n" s="0">
+        <v>100.3</v>
       </c>
     </row>
     <row r="5">
@@ -667,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s" s="0">
         <v>14</v>
@@ -676,255 +673,25 @@
         <v>15</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s" s="0">
         <v>17</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K8" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K9" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K10" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I11" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J11" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K11" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="J12" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="K12" t="s" s="0">
-        <v>17</v>
+      <c r="L5" t="n" s="0">
+        <v>100.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>